<commit_message>
update test case Post
</commit_message>
<xml_diff>
--- a/Test_Mobile_mcovid.xlsx
+++ b/Test_Mobile_mcovid.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AD\Documents\GitHub\ga-mcovid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\ga-mcovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C228AF2-48CF-4AA8-99D0-E6BA9AE2DEA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD3BDD-E355-4965-B3CD-66A605742F98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8E5FA642-1EE3-45B7-86BB-FC07B18340E1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8E5FA642-1EE3-45B7-86BB-FC07B18340E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="2" r:id="rId1"/>
     <sheet name="Signin" sheetId="3" r:id="rId2"/>
     <sheet name="Login" sheetId="1" r:id="rId3"/>
+    <sheet name="Post" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="285">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -920,12 +921,236 @@
   <si>
     <t>23/09/2020</t>
   </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>PO_01</t>
+  </si>
+  <si>
+    <t>PO_02</t>
+  </si>
+  <si>
+    <t>PO_03</t>
+  </si>
+  <si>
+    <t>PO_04</t>
+  </si>
+  <si>
+    <t>PO_05</t>
+  </si>
+  <si>
+    <t>PO_06</t>
+  </si>
+  <si>
+    <t>PO_07</t>
+  </si>
+  <si>
+    <t>PO_08</t>
+  </si>
+  <si>
+    <t>Thao tác khi chưa đăng nhập</t>
+  </si>
+  <si>
+    <t>Xem bài Post</t>
+  </si>
+  <si>
+    <t>1. Chọn chức năng xem bài Post
+2. Kiểm tra màn hình.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Mở app thành công
+2. Có sẵn ít nhất 5 bản ghi trong list Post.
+</t>
+  </si>
+  <si>
+    <t>1. Nhấn vào biểu tượng bình luận
+2. Kiểm tra màn hình</t>
+  </si>
+  <si>
+    <t>Màn hình hiển thị thông báo: Yêu cầu đăng nhập để thực hiện chức năng này.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Mở app thành công
+2. Có sẵn ít nhất 5 bản ghi trong list Post.
+3. Xem được bài Post
+</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra màn hình.
+2. giữ biểu tượng bày tỏ cảm xúc.
+3. Kiểm tra màn hình.
+4. Chọn biểu tượng cảm xúc bất kỳ</t>
+  </si>
+  <si>
+    <t>1. Màn hình hiển thị biểu tượng bày tỏ cảm xúc.
+2. Hiển thị các biểu tượng cảm xúc theo hàng ngang.
+3. Khi chọn biểu tượng màn hình có thay đổi icon giống với biểu tượng đã chọn.
+4. Nhưng không được tính vào CSDL</t>
+  </si>
+  <si>
+    <t>Những bài Post đã có sẵn</t>
+  </si>
+  <si>
+    <t>Bày tỏ cảm xúc
+(Like, Dislike, haha, ...)</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra màn hình.
+2. giữ biểu tượng bày tỏ cảm xúc.
+3. Kiểm tra màn hình.
+4. Chọn biểu tượng cảm xúc bất kỳ
+5. Kiểm tra màn hình</t>
+  </si>
+  <si>
+    <t>1. Màn hình hiển thị biểu tượng bày tỏ cảm xúc.
+2. Hiển thị các biểu tượng cảm xúc theo hàng ngang.
+3. Khi chọn biểu tượng màn hình có thay đổi icon giống với biểu tượng đã chọn.
+4. Khi người dùng chọn xong, các biểu tượng cảm xúc ẩn đi, chỉ hiển thị biểu tượng đã chọn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share </t>
+  </si>
+  <si>
+    <t>1. Kiểm tra màn hình.
+2.Nhấn vào biểu tượng Share 
+3. Kiểm tra màn hình.</t>
+  </si>
+  <si>
+    <t>1. Màn hình có hiển thị biểu tượng share ở dưới bài Post.
+2. Cho phép nhấn vào biểu tượng.
+3. Có thay đổi màu nền của block chứa icon.
+4. Hiển thị thông báo đăng nhập để thực hiện chức năng.</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng nhấn biểu tượng 3 dấu chấm ở góc trên phải bài post</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra màn hình.
+2. Nhấn vào icon dấu 3 chấm dọc ở góc trên phải màn hình.
+3. Kiểm tra màn hình</t>
+  </si>
+  <si>
+    <t>1. Màn hình hiển thị dấu 3 chấm dọc ở góc phải trên bài post.
+2. Cho phép nhấn vào và có thay đổi màu nền.
+3. Show ra 3 chức năng :
+  - Tắt thông báo
+  - Ẩn bài Post
+  - Tắt block và không làm gì cả (trở về màn hình ban đầu khi chưa nhấn vào biểu tượng).</t>
+  </si>
+  <si>
+    <t>Mockup, những bài post có sẵn.</t>
+  </si>
+  <si>
+    <t>PO_09</t>
+  </si>
+  <si>
+    <t>PO_10</t>
+  </si>
+  <si>
+    <t>PO_11</t>
+  </si>
+  <si>
+    <t>Xem được những bài post tồn tại.</t>
+  </si>
+  <si>
+    <t>Xem toàn bộ bài Post</t>
+  </si>
+  <si>
+    <t>Thao tác khi đăng nhập rồi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Mở app thành công.
+2. Đăng nhập thành công.
+2. Có sẵn ít nhất 5 bản ghi trong list Post.
+</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>1. Nhấn vào biểu tượng bình luận
+2. Kiểm tra màn hình.
+3. Nhập bình luận</t>
+  </si>
+  <si>
+    <t>Comment thành công</t>
+  </si>
+  <si>
+    <t>1. Cho phép nhấn vào biểu tượng Commet
+2. Hiển thị chi tiết bình luận
+3. Nhấn vào thanh nhập bình luận thì hiển thì bàn phím để nhập bình luận.
+4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Post interface</t>
+  </si>
+  <si>
+    <t>Kiểm tra giao diện khi mở app thành công</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra màn hình
+2. Kiểm tra giao diện bài Post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Hiển thị những bào Post đã có ở trạng thái Public.
+2. Có avt tác giả, hiển thị thời gian post, dấu 3 chấm dọc, biểu tượng like, comment, share
+</t>
+  </si>
+  <si>
+    <t>Kiểm tra đếm số lượng like, comment, share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Hiển thị những bào Post đã có ở trạng thái Public.
+2. Đếm số lượng bày tỏ cảm xúc đã có.
+3. Đếm đúng số lượng comment đang có.
+4. Đếm số lượt chia sẻ.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Có app đã được cài đặt trong máy
+2. Mở app thành công
+3. Tồn tại ít nhất 1 bản ghi </t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click vào số lượng lượt bày tỏ cảm xúc</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra màn hình
+2. Kiểm tra giao diện bài Post
+3. Nhấp chuột vào số lượng bản ghi.
+4. Quan sát màn hình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Bài Post hiển thị giống với bản design.
+2. Có hiển thị số lượng lượt Like, haha, …
+3. Cho phép nhấp chuột.
+4. Hiển thị chi tiết người dùng nào bày tỏ cảm xúc gì, đếm tổng lượt like, haha, care, love, angry, sad, wow.
+5. Nếu người dùng chưa add friend thì hiện biểu tượng add friend bên cạnh tên người dùng. </t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click
+ vào avt của người comment, bày tỏ cảm xúc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Có app đã được cài đặt trong máy
+2. Mở app thành công
+3. Tồn tại ít nhất 1 bản ghi 
+4. Mở thành công màn hình tổng hợp lượng like, … </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Kiểm tra màn hình
+2. Click vào avt </t>
+  </si>
+  <si>
+    <t>PO_12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1005,8 +1230,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1058,6 +1290,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1378,7 +1616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1552,20 +1790,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1573,18 +1847,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1594,22 +1856,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1621,46 +1916,43 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1984,34 +2276,34 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="18.75">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="62"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A3" s="59" t="s">
+      <c r="B2" s="66"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="60" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A4" s="59" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1">
+      <c r="A4" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="63"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="35" t="s">
         <v>108</v>
       </c>
@@ -2031,29 +2323,29 @@
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
-      <c r="A8" s="62" t="s">
+    <row r="8" spans="1:6" ht="18">
+      <c r="A8" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="62"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A9" s="59" t="s">
+      <c r="B8" s="66"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1">
+      <c r="A9" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="60" t="s">
+      <c r="B9" s="64"/>
+      <c r="C9" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A10" s="59" t="s">
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1">
+      <c r="A10" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="63"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="35" t="s">
         <v>108</v>
       </c>
@@ -2075,29 +2367,29 @@
       </c>
       <c r="F11" s="37"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
-      <c r="A14" s="62" t="s">
+    <row r="14" spans="1:6" ht="18">
+      <c r="A14" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="62"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A15" s="59" t="s">
+      <c r="B14" s="66"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1">
+      <c r="A15" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60" t="s">
+      <c r="B15" s="64"/>
+      <c r="C15" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A16" s="59" t="s">
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1">
+      <c r="A16" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="63"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="35" t="s">
         <v>108</v>
       </c>
@@ -2121,11 +2413,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="A2:B2"/>
@@ -2133,6 +2420,11 @@
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2142,22 +2434,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF24FE9-078F-44AF-9B36-02F3C04AA583}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="92.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="92.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="55" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="56" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="55" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="56" customWidth="1"/>
     <col min="3" max="3" width="23" style="47" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="55" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" style="57" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="57" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" style="47" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="55"/>
-    <col min="13" max="13" width="11.28515625" style="55" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="55"/>
+    <col min="4" max="4" width="16.109375" style="55" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" style="57" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="57" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" style="47" customWidth="1"/>
+    <col min="8" max="12" width="9.109375" style="55"/>
+    <col min="13" max="13" width="11.33203125" style="55" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="54" customFormat="1" ht="42.75" customHeight="1">
@@ -2182,10 +2474,10 @@
       <c r="G1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="64"/>
+      <c r="I1" s="76"/>
       <c r="J1" s="45" t="s">
         <v>7</v>
       </c>
@@ -2223,28 +2515,28 @@
       <c r="N2" s="48"/>
     </row>
     <row r="3" spans="1:14" ht="35.25" customHeight="1">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="77" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
     </row>
     <row r="4" spans="1:14" ht="184.5" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="78" t="s">
         <v>166</v>
       </c>
       <c r="C4" s="47" t="s">
@@ -2275,7 +2567,7 @@
       <c r="A5" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B5" s="71"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="47" t="s">
         <v>165</v>
       </c>
@@ -2300,7 +2592,7 @@
       <c r="A6" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="78" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="46" t="s">
@@ -2326,7 +2618,7 @@
       <c r="A7" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="72"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="47" t="s">
         <v>76</v>
       </c>
@@ -2350,7 +2642,7 @@
       <c r="A8" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B8" s="72"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="51" t="s">
         <v>72</v>
       </c>
@@ -2377,7 +2669,7 @@
       <c r="A9" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="72"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="49" t="s">
         <v>54</v>
       </c>
@@ -2401,14 +2693,14 @@
       <c r="A10" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="72"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="49" t="s">
         <v>55</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="69" t="s">
         <v>182</v>
       </c>
       <c r="H10" s="47"/>
@@ -2425,14 +2717,14 @@
       <c r="A11" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="68" t="s">
+      <c r="B11" s="80"/>
+      <c r="C11" s="74" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="49" t="s">
         <v>208</v>
       </c>
-      <c r="F11" s="67"/>
+      <c r="F11" s="70"/>
       <c r="G11" s="47" t="s">
         <v>193</v>
       </c>
@@ -2444,8 +2736,8 @@
       <c r="A12" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="69"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="75"/>
       <c r="E12" s="49" t="s">
         <v>209</v>
       </c>
@@ -2482,7 +2774,7 @@
       <c r="A14" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="71" t="s">
         <v>187</v>
       </c>
       <c r="C14" s="47" t="s">
@@ -2491,7 +2783,7 @@
       <c r="E14" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="F14" s="66" t="s">
+      <c r="F14" s="69" t="s">
         <v>157</v>
       </c>
       <c r="L14" s="53" t="s">
@@ -2502,14 +2794,14 @@
       <c r="A15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="47" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="F15" s="67"/>
+      <c r="F15" s="70"/>
       <c r="L15" s="53" t="s">
         <v>138</v>
       </c>
@@ -2518,7 +2810,7 @@
       <c r="A16" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B16" s="74"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="49" t="s">
         <v>70</v>
       </c>
@@ -2536,7 +2828,7 @@
       <c r="A17" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="74"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="49" t="s">
         <v>71</v>
       </c>
@@ -2554,7 +2846,7 @@
       <c r="A18" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B18" s="75"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="51" t="s">
         <v>190</v>
       </c>
@@ -2573,7 +2865,7 @@
       <c r="A19" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="71" t="s">
         <v>197</v>
       </c>
       <c r="C19" s="51" t="s">
@@ -2597,7 +2889,7 @@
       <c r="A20" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B20" s="75"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="47" t="s">
         <v>199</v>
       </c>
@@ -2615,7 +2907,7 @@
       <c r="A21" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="71" t="s">
         <v>215</v>
       </c>
       <c r="C21" s="49" t="s">
@@ -2635,14 +2927,14 @@
       <c r="A22" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B22" s="74"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="49" t="s">
         <v>223</v>
       </c>
       <c r="E22" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="F22" s="66" t="s">
+      <c r="F22" s="69" t="s">
         <v>182</v>
       </c>
       <c r="L22" s="53" t="s">
@@ -2653,14 +2945,14 @@
       <c r="A23" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="68" t="s">
+      <c r="B23" s="72"/>
+      <c r="C23" s="74" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="F23" s="67"/>
+      <c r="F23" s="70"/>
       <c r="L23" s="53" t="s">
         <v>138</v>
       </c>
@@ -2669,8 +2961,8 @@
       <c r="A24" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="69"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="75"/>
       <c r="E24" s="49" t="s">
         <v>218</v>
       </c>
@@ -2685,7 +2977,7 @@
       <c r="A25" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B25" s="75"/>
+      <c r="B25" s="73"/>
       <c r="C25" s="51" t="s">
         <v>219</v>
       </c>
@@ -2702,18 +2994,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B12"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="B21:B25"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2725,35 +3017,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDC95F3-AE03-493A-A963-6CC85904072D}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="24" style="3" customWidth="1"/>
-    <col min="5" max="6" width="37.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="37.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="17" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="24.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" style="3" customWidth="1"/>
     <col min="12" max="12" width="12" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="13" max="13" width="14.33203125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
-      <c r="H1" s="82" t="s">
+      <c r="H1" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="94"/>
     </row>
     <row r="2" spans="1:14" s="20" customFormat="1">
       <c r="A2" s="16" t="s">
@@ -2777,10 +3069,10 @@
       <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="64"/>
+      <c r="I2" s="76"/>
       <c r="J2" s="16" t="s">
         <v>7</v>
       </c>
@@ -2817,28 +3109,28 @@
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
     </row>
     <row r="5" spans="1:14" ht="123" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="97" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2860,11 +3152,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="126">
+    <row r="6" spans="1:14" ht="124.8">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="3" t="s">
         <v>41</v>
       </c>
@@ -2881,44 +3173,44 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="63">
+    <row r="7" spans="1:14" ht="62.4">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="85" t="s">
+      <c r="B7" s="97"/>
+      <c r="C7" s="96" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="95" t="s">
         <v>50</v>
       </c>
       <c r="L7" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="63">
+    <row r="8" spans="1:14" ht="62.4">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="85"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="96"/>
       <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="84"/>
+      <c r="F8" s="95"/>
       <c r="L8" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="63">
+    <row r="9" spans="1:14" ht="62.4">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="85"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="96"/>
       <c r="E9" s="3" t="s">
         <v>46</v>
       </c>
@@ -2929,12 +3221,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="63">
+    <row r="10" spans="1:14" ht="62.4">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="85"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="96"/>
       <c r="E10" s="3" t="s">
         <v>47</v>
       </c>
@@ -2945,12 +3237,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="63">
+    <row r="11" spans="1:14" ht="62.4">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="85"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="96"/>
       <c r="E11" s="3" t="s">
         <v>48</v>
       </c>
@@ -2961,11 +3253,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="63">
+    <row r="12" spans="1:14" ht="62.4">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="84" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2981,11 +3273,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="63">
+    <row r="13" spans="1:14" ht="62.4">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="74"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="3" t="s">
         <v>76</v>
       </c>
@@ -2999,11 +3291,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="78.75">
+    <row r="14" spans="1:14" ht="78">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="74"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="6" t="s">
         <v>72</v>
       </c>
@@ -3017,11 +3309,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="78.75">
+    <row r="15" spans="1:14" ht="78">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="14" t="s">
         <v>54</v>
       </c>
@@ -3035,51 +3327,51 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="63">
+    <row r="16" spans="1:14" ht="62.4">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="74"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="80" t="s">
+      <c r="D16" s="99" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="81" t="s">
+      <c r="F16" s="100" t="s">
         <v>62</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="63">
+    <row r="17" spans="1:13" ht="62.4">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="68" t="s">
+      <c r="B17" s="72"/>
+      <c r="C17" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="80"/>
+      <c r="D17" s="99"/>
       <c r="E17" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="81"/>
+      <c r="F17" s="100"/>
       <c r="L17" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="63">
+    <row r="18" spans="1:13" ht="62.4">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="80"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="99"/>
       <c r="E18" s="8" t="s">
         <v>69</v>
       </c>
@@ -3094,7 +3386,7 @@
       <c r="A19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="97" t="s">
         <v>63</v>
       </c>
       <c r="C19" s="15" t="s">
@@ -3103,7 +3395,7 @@
       <c r="E19" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="78" t="s">
+      <c r="F19" s="92" t="s">
         <v>157</v>
       </c>
       <c r="L19" s="19" t="s">
@@ -3114,23 +3406,23 @@
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="76"/>
+      <c r="B20" s="97"/>
       <c r="C20" s="15" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="67"/>
+      <c r="F20" s="70"/>
       <c r="L20" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="31.5">
+    <row r="21" spans="1:13" ht="31.2">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="76"/>
+      <c r="B21" s="97"/>
       <c r="C21" s="14" t="s">
         <v>70</v>
       </c>
@@ -3144,11 +3436,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="31.5">
+    <row r="22" spans="1:13" ht="31.2">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="76"/>
+      <c r="B22" s="97"/>
       <c r="C22" s="14" t="s">
         <v>71</v>
       </c>
@@ -3163,23 +3455,23 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="21" customFormat="1" ht="18.75">
+    <row r="23" spans="1:13" s="21" customFormat="1" ht="17.399999999999999">
       <c r="A23" s="23" t="s">
         <v>85</v>
       </c>
       <c r="B23" s="17"/>
     </row>
-    <row r="24" spans="1:13" ht="47.25">
+    <row r="24" spans="1:13" ht="46.8">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="81" t="s">
         <v>120</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="89" t="s">
+      <c r="D24" s="85" t="s">
         <v>121</v>
       </c>
       <c r="E24" s="27" t="s">
@@ -3195,15 +3487,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="63">
+    <row r="25" spans="1:13" ht="62.4">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="87"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="90"/>
+      <c r="D25" s="86"/>
       <c r="E25" s="24" t="s">
         <v>101</v>
       </c>
@@ -3214,15 +3506,15 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="47.25">
+    <row r="26" spans="1:13" ht="46.8">
       <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="87"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="90"/>
+      <c r="D26" s="86"/>
       <c r="E26" s="25" t="s">
         <v>103</v>
       </c>
@@ -3233,15 +3525,15 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="63">
+    <row r="27" spans="1:13" ht="62.4">
       <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="87"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="90"/>
+      <c r="D27" s="86"/>
       <c r="E27" s="24" t="s">
         <v>117</v>
       </c>
@@ -3252,15 +3544,15 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="31.5">
+    <row r="28" spans="1:13" ht="31.2">
       <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="88"/>
+      <c r="B28" s="83"/>
       <c r="C28" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="91"/>
+      <c r="D28" s="87"/>
       <c r="E28" s="39" t="s">
         <v>118</v>
       </c>
@@ -3271,11 +3563,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="47.25">
+    <row r="29" spans="1:13" ht="46.8">
       <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="77" t="s">
+      <c r="B29" s="84" t="s">
         <v>89</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -3291,45 +3583,45 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="47.25">
+    <row r="30" spans="1:13" ht="46.8">
       <c r="A30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="74"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="41" t="s">
         <v>91</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="92" t="s">
+      <c r="F30" s="88" t="s">
         <v>126</v>
       </c>
       <c r="L30" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="63">
+    <row r="31" spans="1:13" ht="62.4">
       <c r="A31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="74"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="42" t="s">
         <v>92</v>
       </c>
       <c r="E31" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="F31" s="93"/>
+      <c r="F31" s="89"/>
       <c r="L31" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="47.25">
+    <row r="32" spans="1:13" ht="46.8">
       <c r="A32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="74"/>
+      <c r="B32" s="72"/>
       <c r="C32" s="41" t="s">
         <v>93</v>
       </c>
@@ -3343,11 +3635,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="63">
+    <row r="33" spans="1:12" ht="62.4">
       <c r="A33" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="74"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="42" t="s">
         <v>94</v>
       </c>
@@ -3361,11 +3653,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="78.75">
+    <row r="34" spans="1:12" ht="78">
       <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="74"/>
+      <c r="B34" s="72"/>
       <c r="C34" s="42" t="s">
         <v>95</v>
       </c>
@@ -3379,11 +3671,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="63">
+    <row r="35" spans="1:12" ht="62.4">
       <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="75"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="42" t="s">
         <v>129</v>
       </c>
@@ -3397,11 +3689,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="63">
+    <row r="36" spans="1:12" ht="62.4">
       <c r="A36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="94" t="s">
+      <c r="B36" s="90" t="s">
         <v>96</v>
       </c>
       <c r="C36" s="24" t="s">
@@ -3417,11 +3709,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="63">
+    <row r="37" spans="1:12" ht="62.4">
       <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="95"/>
+      <c r="B37" s="91"/>
       <c r="C37" s="24" t="s">
         <v>151</v>
       </c>
@@ -3435,11 +3727,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="63">
+    <row r="38" spans="1:12" ht="62.4">
       <c r="A38" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="95"/>
+      <c r="B38" s="91"/>
       <c r="C38" s="24" t="s">
         <v>97</v>
       </c>
@@ -3453,11 +3745,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="63">
+    <row r="39" spans="1:12" ht="62.4">
       <c r="A39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="95"/>
+      <c r="B39" s="91"/>
       <c r="C39" s="24" t="s">
         <v>143</v>
       </c>
@@ -3471,11 +3763,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="63">
+    <row r="40" spans="1:12" ht="62.4">
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="95"/>
+      <c r="B40" s="91"/>
       <c r="C40" s="24" t="s">
         <v>153</v>
       </c>
@@ -3489,11 +3781,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="63">
+    <row r="41" spans="1:12" ht="62.4">
       <c r="A41" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="95"/>
+      <c r="B41" s="91"/>
       <c r="C41" s="24" t="s">
         <v>145</v>
       </c>
@@ -3507,11 +3799,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="47.25">
+    <row r="42" spans="1:12" ht="46.8">
       <c r="A42" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B42" s="95"/>
+      <c r="B42" s="91"/>
       <c r="C42" s="25" t="s">
         <v>148</v>
       </c>
@@ -3525,11 +3817,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="78.75">
+    <row r="43" spans="1:12" ht="62.4">
       <c r="A43" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="95"/>
+      <c r="B43" s="91"/>
       <c r="C43" s="15" t="s">
         <v>79</v>
       </c>
@@ -3537,18 +3829,18 @@
       <c r="E43" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F43" s="78" t="s">
+      <c r="F43" s="92" t="s">
         <v>156</v>
       </c>
       <c r="L43" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="63">
+    <row r="44" spans="1:12" ht="62.4">
       <c r="A44" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="88"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="15" t="s">
         <v>80</v>
       </c>
@@ -3556,7 +3848,7 @@
       <c r="E44" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F44" s="67"/>
+      <c r="F44" s="70"/>
       <c r="L44" s="19" t="s">
         <v>138</v>
       </c>
@@ -3599,17 +3891,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="B36:B44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="C7:C11"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B12:B18"/>
     <mergeCell ref="F19:F20"/>
@@ -3617,6 +3898,419 @@
     <mergeCell ref="B5:B11"/>
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="F16:F17"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="B36:B44"/>
+    <mergeCell ref="F43:F44"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687972C2-6C3A-4AED-A76E-3130718BE50F}">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="5" max="5" width="34.77734375" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="62" customFormat="1" ht="15.6">
+      <c r="B1" s="61"/>
+      <c r="C1" s="63"/>
+      <c r="H1" s="104" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="93"/>
+      <c r="J1" s="94"/>
+    </row>
+    <row r="2" spans="1:14" s="62" customFormat="1" ht="31.8" customHeight="1">
+      <c r="A2" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="76"/>
+      <c r="J2" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="63" customFormat="1" ht="15.6">
+      <c r="A3" s="107"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+    </row>
+    <row r="4" spans="1:14" s="113" customFormat="1" ht="75" customHeight="1">
+      <c r="A4" s="103" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="106" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="106" t="s">
+        <v>273</v>
+      </c>
+      <c r="F4" s="106" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+    </row>
+    <row r="5" spans="1:14" s="113" customFormat="1" ht="75" customHeight="1">
+      <c r="A5" s="103" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="106" t="s">
+        <v>277</v>
+      </c>
+      <c r="E5" s="106" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="106" t="s">
+        <v>276</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>259</v>
+      </c>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="112"/>
+    </row>
+    <row r="6" spans="1:14" s="113" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A6" s="103" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="105" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" s="106" t="s">
+        <v>277</v>
+      </c>
+      <c r="E6" s="106" t="s">
+        <v>279</v>
+      </c>
+      <c r="F6" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>259</v>
+      </c>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="112"/>
+    </row>
+    <row r="7" spans="1:14" s="113" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A7" s="103" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" s="106" t="s">
+        <v>282</v>
+      </c>
+      <c r="E7" s="106" t="s">
+        <v>283</v>
+      </c>
+      <c r="F7" s="106">
+        <v>1</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>259</v>
+      </c>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="112"/>
+    </row>
+    <row r="8" spans="1:14" ht="58.2" customHeight="1">
+      <c r="A8" s="103" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="108" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="D8" s="106" t="s">
+        <v>243</v>
+      </c>
+      <c r="E8" s="106" t="s">
+        <v>242</v>
+      </c>
+      <c r="F8" s="105" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="57.6">
+      <c r="A9" s="103" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="109"/>
+      <c r="C9" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="D9" s="106" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9" s="106" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="115.2" customHeight="1">
+      <c r="A10" s="103" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="109"/>
+      <c r="C10" s="111" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="106" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" s="106" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" s="106" t="s">
+        <v>248</v>
+      </c>
+      <c r="G10" s="105" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="150" customHeight="1">
+      <c r="A11" s="103" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="109"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="106" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="106" t="s">
+        <v>251</v>
+      </c>
+      <c r="F11" s="106" t="s">
+        <v>252</v>
+      </c>
+      <c r="G11" s="105" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="100.8" customHeight="1">
+      <c r="A12" s="103" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="109"/>
+      <c r="C12" s="110" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="106" t="s">
+        <v>246</v>
+      </c>
+      <c r="E12" s="106" t="s">
+        <v>254</v>
+      </c>
+      <c r="F12" s="106" t="s">
+        <v>255</v>
+      </c>
+      <c r="G12" s="105" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="148.19999999999999" customHeight="1">
+      <c r="A13" s="103" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" s="109"/>
+      <c r="C13" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="106" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" s="106" t="s">
+        <v>257</v>
+      </c>
+      <c r="F13" s="106" t="s">
+        <v>258</v>
+      </c>
+      <c r="G13" s="105" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="77.400000000000006" customHeight="1">
+      <c r="A14" s="103" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C14" s="110" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="106" t="s">
+        <v>266</v>
+      </c>
+      <c r="E14" s="106" t="s">
+        <v>242</v>
+      </c>
+      <c r="F14" s="106" t="s">
+        <v>264</v>
+      </c>
+      <c r="G14" s="105"/>
+    </row>
+    <row r="15" spans="1:14" ht="82.8" customHeight="1">
+      <c r="A15" s="103" t="s">
+        <v>284</v>
+      </c>
+      <c r="C15" s="110" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" s="106" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="106" t="s">
+        <v>268</v>
+      </c>
+      <c r="F15" s="106" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.6">
+      <c r="A16" s="103" t="s">
+        <v>260</v>
+      </c>
+      <c r="F16" s="106"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6">
+      <c r="A17" s="103" t="s">
+        <v>261</v>
+      </c>
+      <c r="F17" s="106"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6">
+      <c r="A18" s="103" t="s">
+        <v>262</v>
+      </c>
+      <c r="F18" s="106"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B8:B13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>